<commit_message>
run evaluation on all datasets for all embedding models
</commit_message>
<xml_diff>
--- a/results/all-MiniLM-L6-v2/PoliTo_evaluation_metrics.xlsx
+++ b/results/all-MiniLM-L6-v2/PoliTo_evaluation_metrics.xlsx
@@ -711,94 +711,94 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.006779661016949151</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01587142857142857</v>
+        <v>0.009490847457627119</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0119</v>
+        <v>0.007900000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.005084745762711865</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02856904761904762</v>
+        <v>0.01333254237288136</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0143</v>
+        <v>0.0074</v>
       </c>
       <c r="I3" t="n">
-        <v>0.006352380952380952</v>
+        <v>0.00429593220338983</v>
       </c>
       <c r="J3" t="n">
-        <v>0.02856904761904762</v>
+        <v>0.01604440677966102</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0104</v>
+        <v>0.0068</v>
       </c>
       <c r="L3" t="n">
-        <v>0.005952380952380952</v>
+        <v>0.004406779661016952</v>
       </c>
       <c r="M3" t="n">
-        <v>0.03333095238095238</v>
+        <v>0.0212420338983051</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0101</v>
+        <v>0.0073</v>
       </c>
       <c r="O3" t="n">
-        <v>0.004761904761904762</v>
+        <v>0.003932203389830509</v>
       </c>
       <c r="P3" t="n">
-        <v>0.03333095238095238</v>
+        <v>0.02643966101694917</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0083</v>
+        <v>0.0068</v>
       </c>
       <c r="R3" t="n">
-        <v>0.004757142857142857</v>
+        <v>0.00372542372881356</v>
       </c>
       <c r="S3" t="n">
-        <v>0.03809285714285714</v>
+        <v>0.02915152542372882</v>
       </c>
       <c r="T3" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0066</v>
       </c>
       <c r="U3" t="n">
-        <v>0.004085714285714286</v>
+        <v>0.003198983050847456</v>
       </c>
       <c r="V3" t="n">
-        <v>0.03809285714285714</v>
+        <v>0.02915152542372882</v>
       </c>
       <c r="W3" t="n">
-        <v>0.0074</v>
+        <v>0.0058</v>
       </c>
       <c r="X3" t="n">
-        <v>0.003571428571428571</v>
+        <v>0.002881355932203391</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03809285714285714</v>
+        <v>0.03028135593220339</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.0065</v>
+        <v>0.0053</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.003171428571428572</v>
+        <v>0.002709152542372881</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.03809285714285714</v>
+        <v>0.03163728813559322</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.0059</v>
+        <v>0.005</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.002857142857142858</v>
+        <v>0.002440677966101697</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.03809285714285714</v>
+        <v>0.03163728813559322</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.0053</v>
+        <v>0.0045</v>
       </c>
     </row>
     <row r="4">
@@ -813,94 +813,94 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.02260536398467439</v>
+        <v>0.02077175697865298</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05894075670498083</v>
+        <v>0.05438646688560499</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0327</v>
+        <v>0.0301</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01700191570881236</v>
+        <v>0.01522988505747075</v>
       </c>
       <c r="G4" t="n">
-        <v>0.08930507662835246</v>
+        <v>0.07971372468527674</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0286</v>
+        <v>0.0256</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01402188697318018</v>
+        <v>0.0127215927750407</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1089276819923372</v>
+        <v>0.09929214559387026</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0248</v>
+        <v>0.0226</v>
       </c>
       <c r="L4" t="n">
-        <v>0.01214080459770124</v>
+        <v>0.0110290093048715</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1267169540229885</v>
+        <v>0.1146563286808983</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0222</v>
+        <v>0.0201</v>
       </c>
       <c r="O4" t="n">
-        <v>0.01068965517241367</v>
+        <v>0.009833059660646185</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1385359674329501</v>
+        <v>0.1274086070060216</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0198</v>
+        <v>0.0183</v>
       </c>
       <c r="R4" t="n">
-        <v>0.009619923371647588</v>
+        <v>0.008958565955117168</v>
       </c>
       <c r="S4" t="n">
-        <v>0.1509293582375479</v>
+        <v>0.1400146893815006</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0181</v>
+        <v>0.0168</v>
       </c>
       <c r="U4" t="n">
-        <v>0.008749137931034587</v>
+        <v>0.008297769567596777</v>
       </c>
       <c r="V4" t="n">
-        <v>0.1601646551724137</v>
+        <v>0.1504344896004382</v>
       </c>
       <c r="W4" t="n">
-        <v>0.0166</v>
+        <v>0.0157</v>
       </c>
       <c r="X4" t="n">
-        <v>0.007986111111111164</v>
+        <v>0.007674808429119205</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.166574856321839</v>
+        <v>0.1589817528735629</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.0152</v>
+        <v>0.0146</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.007474904214559353</v>
+        <v>0.007204652435686599</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.1757277298850575</v>
+        <v>0.1670004378762992</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.0143</v>
+        <v>0.0138</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.007136015325670406</v>
+        <v>0.006788451012588844</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.1870849137931034</v>
+        <v>0.1744882252326209</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.0137</v>
+        <v>0.0131</v>
       </c>
     </row>
     <row r="5">
@@ -915,94 +915,94 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.03362771739130462</v>
+        <v>0.03449279580847142</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0862680027173913</v>
+        <v>0.09254541308882797</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0484</v>
+        <v>0.0503</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02374320652173922</v>
+        <v>0.02416436229564041</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1178803668478261</v>
+        <v>0.1244321981273944</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0395</v>
+        <v>0.0405</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01911898777173892</v>
+        <v>0.01937677194003984</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1403376358695652</v>
+        <v>0.1465418134187142</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0337</v>
+        <v>0.0342</v>
       </c>
       <c r="L5" t="n">
-        <v>0.01610054347826073</v>
+        <v>0.01630766991704432</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1558837975543478</v>
+        <v>0.1625105661475732</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0292</v>
+        <v>0.0296</v>
       </c>
       <c r="O5" t="n">
-        <v>0.01408967391304325</v>
+        <v>0.01429583272692024</v>
       </c>
       <c r="P5" t="n">
-        <v>0.1707080842391305</v>
+        <v>0.1770241109979094</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.026</v>
+        <v>0.0265</v>
       </c>
       <c r="R5" t="n">
-        <v>0.01260526494565215</v>
+        <v>0.01278944840634468</v>
       </c>
       <c r="S5" t="n">
-        <v>0.1817484375000001</v>
+        <v>0.1888666909231984</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0236</v>
+        <v>0.024</v>
       </c>
       <c r="U5" t="n">
-        <v>0.01141946331521748</v>
+        <v>0.01157905205452986</v>
       </c>
       <c r="V5" t="n">
-        <v>0.1923627038043481</v>
+        <v>0.1982558773589424</v>
       </c>
       <c r="W5" t="n">
-        <v>0.0216</v>
+        <v>0.0219</v>
       </c>
       <c r="X5" t="n">
-        <v>0.01044497282608682</v>
+        <v>0.01061951195847413</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.2005824388586959</v>
+        <v>0.2070009120457907</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.0199</v>
+        <v>0.0202</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.009728294836956699</v>
+        <v>0.00985522728375234</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.2096175271739133</v>
+        <v>0.2156776791345215</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.0186</v>
+        <v>0.0188</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.009103260869565068</v>
+        <v>0.009199049143745064</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.2171480298913047</v>
+        <v>0.2227455683306602</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.0175</v>
+        <v>0.0177</v>
       </c>
     </row>
     <row r="6">
@@ -1017,94 +1017,94 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.03697478991596641</v>
+        <v>0.01794258373205739</v>
       </c>
       <c r="D6" t="n">
-        <v>0.06979915966386553</v>
+        <v>0.03926782296650717</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0483</v>
+        <v>0.0246</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02100840336134455</v>
+        <v>0.01244019138755979</v>
       </c>
       <c r="G6" t="n">
-        <v>0.07408067226890755</v>
+        <v>0.05150705741626794</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0327</v>
+        <v>0.02</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01625042016806722</v>
+        <v>0.01108887559808614</v>
       </c>
       <c r="J6" t="n">
-        <v>0.08913697478991595</v>
+        <v>0.06802775119617227</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0275</v>
+        <v>0.0191</v>
       </c>
       <c r="L6" t="n">
-        <v>0.01344537815126051</v>
+        <v>0.009449760765550217</v>
       </c>
       <c r="M6" t="n">
-        <v>0.09663949579831929</v>
+        <v>0.07676255980861246</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0236</v>
+        <v>0.0168</v>
       </c>
       <c r="O6" t="n">
-        <v>0.01109243697478992</v>
+        <v>0.008325358851674647</v>
       </c>
       <c r="P6" t="n">
-        <v>0.09874033613445375</v>
+        <v>0.08421925837320576</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0199</v>
+        <v>0.0152</v>
       </c>
       <c r="R6" t="n">
-        <v>0.009800000000000001</v>
+        <v>0.007570215311004771</v>
       </c>
       <c r="S6" t="n">
-        <v>0.1057428571428571</v>
+        <v>0.09297404306220099</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0179</v>
+        <v>0.014</v>
       </c>
       <c r="U6" t="n">
-        <v>0.008886554621848737</v>
+        <v>0.007284210526315784</v>
       </c>
       <c r="V6" t="n">
-        <v>0.1127453781512605</v>
+        <v>0.1038382775119617</v>
       </c>
       <c r="W6" t="n">
-        <v>0.0165</v>
+        <v>0.0136</v>
       </c>
       <c r="X6" t="n">
-        <v>0.007983193277310929</v>
+        <v>0.00681818181818183</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.113946218487395</v>
+        <v>0.1085290669856459</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.0149</v>
+        <v>0.0128</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.00764873949579832</v>
+        <v>0.006267224880382781</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.1195487394957983</v>
+        <v>0.1118916267942584</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.0144</v>
+        <v>0.0119</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.007058823529411768</v>
+        <v>0.005956937799043043</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.1279521008403361</v>
+        <v>0.1177212918660287</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.0134</v>
+        <v>0.0113</v>
       </c>
     </row>
     <row r="7">
@@ -1119,94 +1119,94 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.03340380549682871</v>
+        <v>0.03911862360398465</v>
       </c>
       <c r="D7" t="n">
-        <v>0.07844101479915434</v>
+        <v>0.0931254452158165</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0469</v>
+        <v>0.0551</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0238900634249471</v>
+        <v>0.02629037126471465</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1130980972515856</v>
+        <v>0.1241651373377604</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0394</v>
+        <v>0.0434</v>
       </c>
       <c r="I7" t="n">
-        <v>0.01889281183932349</v>
+        <v>0.02049166918200999</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1279849894291755</v>
+        <v>0.1432637186839723</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0329</v>
+        <v>0.0359</v>
       </c>
       <c r="L7" t="n">
-        <v>0.01575052854122618</v>
+        <v>0.0170691216420161</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1386264270613108</v>
+        <v>0.1581334138243285</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0283</v>
+        <v>0.0308</v>
       </c>
       <c r="O7" t="n">
-        <v>0.01344608879492601</v>
+        <v>0.01494717778448511</v>
       </c>
       <c r="P7" t="n">
-        <v>0.1441921775898521</v>
+        <v>0.1716805010564444</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0246</v>
+        <v>0.0275</v>
       </c>
       <c r="R7" t="n">
-        <v>0.01204376321353064</v>
+        <v>0.01323290069423468</v>
       </c>
       <c r="S7" t="n">
-        <v>0.1574260042283299</v>
+        <v>0.1819545427105345</v>
       </c>
       <c r="T7" t="n">
+        <v>0.0247</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.0119244793238756</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.1911020525203745</v>
+      </c>
+      <c r="W7" t="n">
         <v>0.0224</v>
       </c>
-      <c r="U7" t="n">
-        <v>0.01087801268498942</v>
-      </c>
-      <c r="V7" t="n">
-        <v>0.1661342494714588</v>
-      </c>
-      <c r="W7" t="n">
-        <v>0.0204</v>
-      </c>
       <c r="X7" t="n">
-        <v>0.01009513742071882</v>
+        <v>0.01091910654995452</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.1738357293868922</v>
+        <v>0.1994616057953519</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.0191</v>
+        <v>0.0207</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.009668710359408058</v>
+        <v>0.0102063990341082</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.1847232558139535</v>
+        <v>0.2081108662843348</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.0184</v>
+        <v>0.0195</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.009344608879492591</v>
+        <v>0.009574403863567602</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.1983847780126849</v>
+        <v>0.2155690310896472</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.0178</v>
+        <v>0.0183</v>
       </c>
     </row>
     <row r="8">
@@ -1221,94 +1221,94 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.02051860202931225</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0544968253968254</v>
+        <v>0.05735682074408118</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0282</v>
+        <v>0.0302</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01825396825396826</v>
+        <v>0.01781285231116117</v>
       </c>
       <c r="G8" t="n">
-        <v>0.09942380952380953</v>
+        <v>0.09839797068771139</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0308</v>
+        <v>0.0302</v>
       </c>
       <c r="I8" t="n">
-        <v>0.01428968253968254</v>
+        <v>0.01391014656144312</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1205873015873016</v>
+        <v>0.1187580608793686</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0256</v>
+        <v>0.0249</v>
       </c>
       <c r="L8" t="n">
-        <v>0.01150793650793651</v>
+        <v>0.0120631341600902</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1311690476190476</v>
+        <v>0.1372001127395715</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0212</v>
+        <v>0.0222</v>
       </c>
       <c r="O8" t="n">
-        <v>0.01142857142857143</v>
+        <v>0.01091319052987596</v>
       </c>
       <c r="P8" t="n">
-        <v>0.1695285714285714</v>
+        <v>0.1564723788049605</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.0214</v>
+        <v>0.0204</v>
       </c>
       <c r="R8" t="n">
-        <v>0.009517460317460322</v>
+        <v>0.009725930101465597</v>
       </c>
       <c r="S8" t="n">
-        <v>0.1695285714285714</v>
+        <v>0.1640951521984216</v>
       </c>
       <c r="T8" t="n">
-        <v>0.018</v>
+        <v>0.0184</v>
       </c>
       <c r="U8" t="n">
-        <v>0.008848412698412694</v>
+        <v>0.00886426155580608</v>
       </c>
       <c r="V8" t="n">
-        <v>0.1801111111111111</v>
+        <v>0.1722209695603156</v>
       </c>
       <c r="W8" t="n">
         <v>0.0169</v>
       </c>
       <c r="X8" t="n">
-        <v>0.008134920634920637</v>
+        <v>0.008483652762119532</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.1836825396825397</v>
+        <v>0.1872085682074408</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.0156</v>
+        <v>0.0162</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.008105555555555557</v>
+        <v>0.007884554678692221</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.2006896825396826</v>
+        <v>0.1950735062006765</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.0156</v>
+        <v>0.0152</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.007777777777777781</v>
+        <v>0.007418263810597478</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.2082952380952381</v>
+        <v>0.1999580608793687</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.015</v>
+        <v>0.0143</v>
       </c>
     </row>
     <row r="9">
@@ -1323,94 +1323,94 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.02550335570469799</v>
+        <v>0.03349282296650714</v>
       </c>
       <c r="D9" t="n">
-        <v>0.06599530201342281</v>
+        <v>0.08579789473684209</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0368</v>
+        <v>0.0482</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01879194630872484</v>
+        <v>0.02315789473684216</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1011181208053692</v>
+        <v>0.1153822009569377</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0317</v>
+        <v>0.0386</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0143248322147651</v>
+        <v>0.01838000000000011</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1093476510067114</v>
+        <v>0.1338054545454545</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0253</v>
+        <v>0.0323</v>
       </c>
       <c r="L9" t="n">
-        <v>0.01208053691275168</v>
+        <v>0.01545454545454552</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1205328859060403</v>
+        <v>0.1454014354066986</v>
       </c>
       <c r="N9" t="n">
-        <v>0.022</v>
+        <v>0.0279</v>
       </c>
       <c r="O9" t="n">
-        <v>0.01181208053691276</v>
+        <v>0.01381818181818172</v>
       </c>
       <c r="P9" t="n">
-        <v>0.1462597315436241</v>
+        <v>0.1613182775119617</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0219</v>
+        <v>0.0255</v>
       </c>
       <c r="R9" t="n">
-        <v>0.0109530201342282</v>
+        <v>0.01255971291866034</v>
       </c>
       <c r="S9" t="n">
-        <v>0.1627026845637584</v>
+        <v>0.1747973205741628</v>
       </c>
       <c r="T9" t="n">
-        <v>0.0205</v>
+        <v>0.0234</v>
       </c>
       <c r="U9" t="n">
-        <v>0.009979194630872476</v>
+        <v>0.01159933014354076</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1679597315436241</v>
+        <v>0.1843448803827752</v>
       </c>
       <c r="W9" t="n">
-        <v>0.0188</v>
+        <v>0.0218</v>
       </c>
       <c r="X9" t="n">
-        <v>0.00939597315436241</v>
+        <v>0.01069377990430628</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.178586577181208</v>
+        <v>0.1937321531100479</v>
       </c>
       <c r="Z9" t="n">
+        <v>0.0203</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0.009900669856459305</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.2014115789473685</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.0189</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.009339712918660203</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0.2091786602870815</v>
+      </c>
+      <c r="AF9" t="n">
         <v>0.0179</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>0.008939597315436242</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>0.1855214765100671</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>0.0171</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>0.008590604026845642</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>0.1939107382550336</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>0.0165</v>
       </c>
     </row>
     <row r="10">
@@ -1425,94 +1425,94 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.02415458937198065</v>
+        <v>0.02226310947562116</v>
       </c>
       <c r="D10" t="n">
-        <v>0.03734106280193236</v>
+        <v>0.03262840386384544</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0293</v>
+        <v>0.0265</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01610305958132042</v>
+        <v>0.01593836246550146</v>
       </c>
       <c r="G10" t="n">
-        <v>0.04849130434782609</v>
+        <v>0.046593169273229</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0242</v>
+        <v>0.0238</v>
       </c>
       <c r="I10" t="n">
-        <v>0.01320982286634461</v>
+        <v>0.01302263109475607</v>
       </c>
       <c r="J10" t="n">
-        <v>0.05901062801932366</v>
+        <v>0.05677559797608089</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0216</v>
+        <v>0.0212</v>
       </c>
       <c r="L10" t="n">
-        <v>0.01135265700483089</v>
+        <v>0.01130404783808637</v>
       </c>
       <c r="M10" t="n">
-        <v>0.068175845410628</v>
+        <v>0.0658000689972401</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0195</v>
+        <v>0.0193</v>
       </c>
       <c r="O10" t="n">
-        <v>0.01004830917874397</v>
+        <v>0.01016559337626479</v>
       </c>
       <c r="P10" t="n">
-        <v>0.07452576489533011</v>
+        <v>0.07420772769089232</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.0177</v>
+        <v>0.0179</v>
       </c>
       <c r="R10" t="n">
-        <v>0.009171980676328489</v>
+        <v>0.0093002299908003</v>
       </c>
       <c r="S10" t="n">
-        <v>0.08070885668276974</v>
+        <v>0.08122976080956755</v>
       </c>
       <c r="T10" t="n">
-        <v>0.0165</v>
+        <v>0.0167</v>
       </c>
       <c r="U10" t="n">
-        <v>0.008609822866344598</v>
+        <v>0.00865982060717572</v>
       </c>
       <c r="V10" t="n">
-        <v>0.08952898550724642</v>
+        <v>0.08730929162833476</v>
       </c>
       <c r="W10" t="n">
-        <v>0.0157</v>
+        <v>0.0158</v>
       </c>
       <c r="X10" t="n">
-        <v>0.008212560386473436</v>
+        <v>0.008078426862925332</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.09730305958132049</v>
+        <v>0.09297316007359695</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.0151</v>
+        <v>0.0149</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.007757809983896957</v>
+        <v>0.007557106715731531</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.1036099838969405</v>
+        <v>0.0987933532658692</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.0144</v>
+        <v>0.014</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.007310789049919476</v>
+        <v>0.007138914443422136</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.1085484702093399</v>
+        <v>0.1030928012879483</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.0137</v>
+        <v>0.0134</v>
       </c>
     </row>
     <row r="11">
@@ -1527,94 +1527,94 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.03788968824940044</v>
+        <v>0.03605884365378067</v>
       </c>
       <c r="D11" t="n">
-        <v>0.06755131894484413</v>
+        <v>0.06062319534724595</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0485</v>
+        <v>0.0452</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02613908872901674</v>
+        <v>0.0257612042422169</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09077146282973625</v>
+        <v>0.08538029421826882</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0406</v>
+        <v>0.0396</v>
       </c>
       <c r="I11" t="n">
-        <v>0.02159016786570746</v>
+        <v>0.02144642490591829</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1080592326139089</v>
+        <v>0.1055439958946288</v>
       </c>
       <c r="K11" t="n">
-        <v>0.036</v>
+        <v>0.0356</v>
       </c>
       <c r="L11" t="n">
-        <v>0.01906474820143881</v>
+        <v>0.01845706465959609</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1255539568345324</v>
+        <v>0.1196425590147109</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0331</v>
+        <v>0.032</v>
       </c>
       <c r="O11" t="n">
-        <v>0.01649880095923262</v>
+        <v>0.01628463906944894</v>
       </c>
       <c r="P11" t="n">
-        <v>0.1322146282973622</v>
+        <v>0.1319596989394457</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0293</v>
+        <v>0.029</v>
       </c>
       <c r="R11" t="n">
-        <v>0.01469928057553954</v>
+        <v>0.01483934314060878</v>
       </c>
       <c r="S11" t="n">
-        <v>0.141873860911271</v>
+        <v>0.1427901128977078</v>
       </c>
       <c r="T11" t="n">
-        <v>0.0266</v>
+        <v>0.0269</v>
       </c>
       <c r="U11" t="n">
-        <v>0.01418968824940047</v>
+        <v>0.0136516250427642</v>
       </c>
       <c r="V11" t="n">
-        <v>0.1568997601918466</v>
+        <v>0.1512129661306876</v>
       </c>
       <c r="W11" t="n">
-        <v>0.026</v>
+        <v>0.025</v>
       </c>
       <c r="X11" t="n">
-        <v>0.01330935251798563</v>
+        <v>0.01260691070817629</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.164895923261391</v>
+        <v>0.1584611358193636</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.0246</v>
+        <v>0.0234</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.01245923261390889</v>
+        <v>0.01176647280191605</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.173232134292566</v>
+        <v>0.1667782757440985</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.0232</v>
+        <v>0.022</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.01213429256594721</v>
+        <v>0.01116660964762215</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.1913928057553957</v>
+        <v>0.1758894970920287</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.0228</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="12">
@@ -1625,94 +1625,94 @@
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
-        <v>0.02427307386862818</v>
+        <v>0.02314387992653368</v>
       </c>
       <c r="D12" t="n">
-        <v>0.05347048716138453</v>
+        <v>0.05252223103063984</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0331</v>
+        <v>0.03181</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0174455461413683</v>
+        <v>0.01658798695238191</v>
       </c>
       <c r="G12" t="n">
-        <v>0.07627379581224604</v>
+        <v>0.07389042950757278</v>
       </c>
       <c r="H12" t="n">
-        <v>0.02818</v>
+        <v>0.02691</v>
       </c>
       <c r="I12" t="n">
-        <v>0.01380509931911905</v>
+        <v>0.01347340442606841</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0891961142927287</v>
+        <v>0.08880529449679228</v>
       </c>
       <c r="K12" t="n">
-        <v>0.02378</v>
+        <v>0.02326</v>
       </c>
       <c r="L12" t="n">
-        <v>0.01173955143477875</v>
+        <v>0.01155411334028173</v>
       </c>
       <c r="M12" t="n">
-        <v>0.09966293625881673</v>
+        <v>0.1001349078517939</v>
       </c>
       <c r="N12" t="n">
-        <v>0.02092</v>
+        <v>0.0206</v>
       </c>
       <c r="O12" t="n">
-        <v>0.01038675217205384</v>
+        <v>0.01025152372073281</v>
       </c>
       <c r="P12" t="n">
-        <v>0.1108036213942227</v>
+        <v>0.1110730221397791</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.01889</v>
+        <v>0.01871</v>
       </c>
       <c r="R12" t="n">
-        <v>0.009316783609152978</v>
+        <v>0.009270177024704987</v>
       </c>
       <c r="S12" t="n">
-        <v>0.1188753487837963</v>
+        <v>0.1195873837981023</v>
       </c>
       <c r="T12" t="n">
-        <v>0.01721</v>
+        <v>0.01715</v>
       </c>
       <c r="U12" t="n">
-        <v>0.008564600128383476</v>
+        <v>0.008505953187245223</v>
       </c>
       <c r="V12" t="n">
-        <v>0.1263999432096166</v>
+        <v>0.1267870330117559</v>
       </c>
       <c r="W12" t="n">
-        <v>0.01599</v>
+        <v>0.01589</v>
       </c>
       <c r="X12" t="n">
-        <v>0.007913364990039841</v>
+        <v>0.007877573492546051</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.1317500199904139</v>
+        <v>0.1336629710843004</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.01488</v>
+        <v>0.01484</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.007495427294694863</v>
+        <v>0.007335146022910191</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.1390763386750836</v>
+        <v>0.139637461238302</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.01419</v>
+        <v>0.01391</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.007131331488177279</v>
+        <v>0.006902302060534822</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.1470809931995294</v>
+        <v>0.1450280424200978</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.01357</v>
+        <v>0.01315</v>
       </c>
     </row>
   </sheetData>
@@ -1898,94 +1898,94 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.009302325581395349</v>
+        <v>0.006644518272425248</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01550232558139535</v>
+        <v>0.009301661129568106</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0116</v>
+        <v>0.0078</v>
       </c>
       <c r="E2" t="n">
-        <v>0.009302325581395349</v>
+        <v>0.004983388704318937</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0279046511627907</v>
+        <v>0.01306677740863788</v>
       </c>
       <c r="G2" t="n">
-        <v>0.014</v>
+        <v>0.0072</v>
       </c>
       <c r="H2" t="n">
-        <v>0.006204651162790697</v>
+        <v>0.004210299003322259</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0279046511627907</v>
+        <v>0.01572458471760798</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0102</v>
+        <v>0.0066</v>
       </c>
       <c r="K2" t="n">
-        <v>0.005813953488372093</v>
+        <v>0.004318936877076415</v>
       </c>
       <c r="L2" t="n">
-        <v>0.03255581395348837</v>
+        <v>0.0208186046511628</v>
       </c>
       <c r="M2" t="n">
-        <v>0.009900000000000001</v>
+        <v>0.0072</v>
       </c>
       <c r="N2" t="n">
-        <v>0.004651162790697674</v>
+        <v>0.003853820598006646</v>
       </c>
       <c r="O2" t="n">
-        <v>0.03255581395348837</v>
+        <v>0.02591262458471762</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0081</v>
+        <v>0.0067</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.004646511627906977</v>
+        <v>0.003651162790697675</v>
       </c>
       <c r="R2" t="n">
-        <v>0.03720697674418604</v>
+        <v>0.02857043189368771</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0083</v>
+        <v>0.0065</v>
       </c>
       <c r="T2" t="n">
-        <v>0.003990697674418606</v>
+        <v>0.003135215946843852</v>
       </c>
       <c r="U2" t="n">
-        <v>0.03720697674418604</v>
+        <v>0.02857043189368771</v>
       </c>
       <c r="V2" t="n">
-        <v>0.0072</v>
+        <v>0.0057</v>
       </c>
       <c r="W2" t="n">
-        <v>0.003488372093023256</v>
+        <v>0.002823920265780732</v>
       </c>
       <c r="X2" t="n">
-        <v>0.03720697674418604</v>
+        <v>0.02967774086378738</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.0064</v>
+        <v>0.0052</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.003097674418604651</v>
+        <v>0.00265514950166113</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.03720697674418604</v>
+        <v>0.03100664451827243</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.0057</v>
+        <v>0.0049</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.002790697674418605</v>
+        <v>0.002392026578073091</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.03720697674418604</v>
+        <v>0.03100664451827243</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.0052</v>
+        <v>0.0044</v>
       </c>
     </row>
     <row r="3">
@@ -1995,94 +1995,94 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0290540540540541</v>
+        <v>0.02880013625138615</v>
       </c>
       <c r="C3" t="n">
-        <v>0.07492871621621627</v>
+        <v>0.07671382099974391</v>
       </c>
       <c r="D3" t="n">
         <v>0.0419</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0209459459459457</v>
+        <v>0.02045757756394119</v>
       </c>
       <c r="F3" t="n">
-        <v>0.106023211446741</v>
+        <v>0.1058791535382748</v>
       </c>
       <c r="G3" t="n">
-        <v>0.035</v>
+        <v>0.0343</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01700397456279782</v>
+        <v>0.01661563484629272</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1273042527821942</v>
+        <v>0.1269386130744521</v>
       </c>
       <c r="J3" t="n">
-        <v>0.03</v>
+        <v>0.0294</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01445747217806012</v>
+        <v>0.01411763036135201</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1437811804451514</v>
+        <v>0.1426565386471346</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0263</v>
+        <v>0.0257</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01267885532591392</v>
+        <v>0.0124442930540196</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1573584459459463</v>
+        <v>0.156439359618494</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0235</v>
+        <v>0.0231</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.01136651430842577</v>
+        <v>0.01120007096426199</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1689602344992056</v>
+        <v>0.1685987056118522</v>
       </c>
       <c r="S3" t="n">
-        <v>0.0213</v>
+        <v>0.021</v>
       </c>
       <c r="T3" t="n">
-        <v>0.01031142686804432</v>
+        <v>0.01021769564847081</v>
       </c>
       <c r="U3" t="n">
-        <v>0.1790023052464235</v>
+        <v>0.1784154787249129</v>
       </c>
       <c r="V3" t="n">
-        <v>0.0195</v>
+        <v>0.0193</v>
       </c>
       <c r="W3" t="n">
-        <v>0.00942468203497589</v>
+        <v>0.009397797269294834</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1864711844197144</v>
+        <v>0.1870784609270763</v>
       </c>
       <c r="Y3" t="n">
         <v>0.0179</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.008793263116057262</v>
+        <v>0.008755542308892628</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.1955551470588242</v>
+        <v>0.1954821993244195</v>
       </c>
       <c r="AB3" t="n">
         <v>0.0168</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.008286963434022358</v>
+        <v>0.008198927020353027</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.2046735095389514</v>
+        <v>0.2027242981634445</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.0159</v>
+        <v>0.0158</v>
       </c>
     </row>
     <row r="4">
@@ -2092,94 +2092,94 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03412162162162156</v>
+        <v>0.03485177151120762</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07670388513513515</v>
+        <v>0.08227343938298386</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0472</v>
+        <v>0.049</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02331081081081076</v>
+        <v>0.02349963846710031</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1052550675675676</v>
+        <v>0.1095249457700651</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0382</v>
+        <v>0.0387</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01836165540540547</v>
+        <v>0.01859705953241719</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1201760135135135</v>
+        <v>0.1281040973728609</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0319</v>
+        <v>0.0325</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01528716216216216</v>
+        <v>0.01553386358158568</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1301864864864865</v>
+        <v>0.141737647625934</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0274</v>
+        <v>0.028</v>
       </c>
       <c r="N4" t="n">
-        <v>0.01297297297297298</v>
+        <v>0.01361291877560835</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1350557432432432</v>
+        <v>0.1540575560375996</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0237</v>
+        <v>0.025</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.01159273648648646</v>
+        <v>0.01209190166305111</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1470369932432432</v>
+        <v>0.164025476018318</v>
       </c>
       <c r="S4" t="n">
-        <v>0.0215</v>
+        <v>0.0225</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0104777027027027</v>
+        <v>0.01098949144372125</v>
       </c>
       <c r="U4" t="n">
-        <v>0.1554023648648648</v>
+        <v>0.1735188961195473</v>
       </c>
       <c r="V4" t="n">
-        <v>0.0196</v>
+        <v>0.0207</v>
       </c>
       <c r="W4" t="n">
-        <v>0.009670608108108124</v>
+        <v>0.01009279344420319</v>
       </c>
       <c r="X4" t="n">
-        <v>0.1617971283783783</v>
+        <v>0.1811392142684989</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.0183</v>
+        <v>0.0191</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.00926266891891893</v>
+        <v>0.009412677753675672</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.1716222972972972</v>
+        <v>0.1887232345143414</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.0176</v>
+        <v>0.0179</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.008885135135135105</v>
+        <v>0.008845504940949609</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.184226858108108</v>
+        <v>0.1958532658471928</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.017</v>
+        <v>0.0169</v>
       </c>
     </row>
     <row r="5">
@@ -2189,94 +2189,94 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.02254545454545456</v>
+        <v>0.02753623188405807</v>
       </c>
       <c r="C5" t="n">
-        <v>0.06072690909090909</v>
+        <v>0.07274032091097306</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0329</v>
+        <v>0.0399</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01854545454545454</v>
+        <v>0.02070393374741214</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1003418181818182</v>
+        <v>0.1075845755693582</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0313</v>
+        <v>0.0347</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01430872727272727</v>
+        <v>0.01632784679089038</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1144974545454545</v>
+        <v>0.126897049689441</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0254</v>
+        <v>0.0289</v>
       </c>
       <c r="K5" t="n">
-        <v>0.01181818181818181</v>
+        <v>0.01389751552795042</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1254061818181818</v>
+        <v>0.1416361283643893</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0216</v>
+        <v>0.0253</v>
       </c>
       <c r="N5" t="n">
-        <v>0.01163636363636364</v>
+        <v>0.0124844720496893</v>
       </c>
       <c r="O5" t="n">
-        <v>0.1569210909090909</v>
+        <v>0.1590934782608697</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0217</v>
+        <v>0.0232</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.01029527272727274</v>
+        <v>0.01125869565217401</v>
       </c>
       <c r="R5" t="n">
-        <v>0.1658301818181818</v>
+        <v>0.1698838509316771</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0194</v>
+        <v>0.0211</v>
       </c>
       <c r="T5" t="n">
-        <v>0.009461090909090898</v>
+        <v>0.01034363354037279</v>
       </c>
       <c r="U5" t="n">
-        <v>0.1735272727272728</v>
+        <v>0.1787786749482403</v>
       </c>
       <c r="V5" t="n">
-        <v>0.0179</v>
+        <v>0.0196</v>
       </c>
       <c r="W5" t="n">
-        <v>0.008818181818181805</v>
+        <v>0.009679089026915126</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1809214545454546</v>
+        <v>0.1907371118012423</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.0168</v>
+        <v>0.0184</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.008557454545454557</v>
+        <v>0.008975051759834363</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.1924712727272728</v>
+        <v>0.1985017080745343</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.0164</v>
+        <v>0.0172</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.008218181818181824</v>
+        <v>0.00845755693581769</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.2005014545454546</v>
+        <v>0.2049453933747414</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.0158</v>
+        <v>0.0162</v>
       </c>
     </row>
     <row r="6">
@@ -2286,94 +2286,94 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0296724470134874</v>
+        <v>0.027809104662357</v>
       </c>
       <c r="C6" t="n">
-        <v>0.04947755298651254</v>
+        <v>0.04388253335167098</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0371</v>
+        <v>0.034</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02013487475915223</v>
+        <v>0.01988722321551327</v>
       </c>
       <c r="F6" t="n">
-        <v>0.06547668593448944</v>
+        <v>0.06218590290193922</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0308</v>
+        <v>0.0301</v>
       </c>
       <c r="H6" t="n">
-        <v>0.01657649325626213</v>
+        <v>0.01640906340255782</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0787151252408478</v>
+        <v>0.07638088295970302</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0274</v>
+        <v>0.027</v>
       </c>
       <c r="K6" t="n">
-        <v>0.01445086705202317</v>
+        <v>0.01417961765919363</v>
       </c>
       <c r="L6" t="n">
-        <v>0.09122658959537572</v>
+        <v>0.08744517948012691</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0249</v>
+        <v>0.0244</v>
       </c>
       <c r="N6" t="n">
-        <v>0.01263969171483615</v>
+        <v>0.01262549855590732</v>
       </c>
       <c r="O6" t="n">
-        <v>0.09770134874759151</v>
+        <v>0.09742448081419387</v>
       </c>
       <c r="P6" t="n">
         <v>0.0224</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.01139248554913298</v>
+        <v>0.01152699766194424</v>
       </c>
       <c r="R6" t="n">
-        <v>0.1052809248554913</v>
+        <v>0.1059775134094353</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0206</v>
+        <v>0.0208</v>
       </c>
       <c r="T6" t="n">
-        <v>0.01085144508670527</v>
+        <v>0.01066656580937943</v>
       </c>
       <c r="U6" t="n">
-        <v>0.1165941233140655</v>
+        <v>0.1129990785311518</v>
       </c>
       <c r="V6" t="n">
-        <v>0.0199</v>
+        <v>0.0195</v>
       </c>
       <c r="W6" t="n">
-        <v>0.01026011560693647</v>
+        <v>0.009898913491954211</v>
       </c>
       <c r="X6" t="n">
-        <v>0.1244574181117533</v>
+        <v>0.1192998487140704</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.019</v>
+        <v>0.0183</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.009646531791907498</v>
+        <v>0.009249305460046646</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.1315795761078998</v>
+        <v>0.1261238344106733</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.018</v>
+        <v>0.0172</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.009248554913294722</v>
+        <v>0.008758080044010779</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.1418298651252409</v>
+        <v>0.1323576536927529</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.0174</v>
+        <v>0.0164</v>
       </c>
     </row>
   </sheetData>
@@ -2559,94 +2559,94 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02335025380710673</v>
+        <v>0.02095394577876502</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05462937394247033</v>
+        <v>0.0493154351713144</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0327</v>
+        <v>0.0294</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01702199661590539</v>
+        <v>0.0153723481370513</v>
       </c>
       <c r="F2" t="n">
-        <v>0.08051610829103203</v>
+        <v>0.07239268351616547</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0281</v>
+        <v>0.0254</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01394764805414548</v>
+        <v>0.01276614314019208</v>
       </c>
       <c r="I2" t="n">
-        <v>0.09810081218274103</v>
+        <v>0.08990112115208121</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0244</v>
+        <v>0.0224</v>
       </c>
       <c r="K2" t="n">
-        <v>0.01199661590524539</v>
+        <v>0.01106412796597953</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1133501184433163</v>
+        <v>0.1037928574880394</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0217</v>
+        <v>0.02</v>
       </c>
       <c r="N2" t="n">
-        <v>0.01059898477157345</v>
+        <v>0.009885468515923071</v>
       </c>
       <c r="O2" t="n">
-        <v>0.124756108291032</v>
+        <v>0.1156940849562634</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0195</v>
+        <v>0.0182</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.009525414551607544</v>
+        <v>0.009004561929154208</v>
       </c>
       <c r="R2" t="n">
-        <v>0.1350946531302875</v>
+        <v>0.1267539941042837</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0178</v>
+        <v>0.0168</v>
       </c>
       <c r="T2" t="n">
-        <v>0.008726666666666785</v>
+        <v>0.008354772145170214</v>
       </c>
       <c r="U2" t="n">
-        <v>0.1442071065989847</v>
+        <v>0.1361784226550006</v>
       </c>
       <c r="V2" t="n">
-        <v>0.0165</v>
+        <v>0.0157</v>
       </c>
       <c r="W2" t="n">
-        <v>0.008037225042301125</v>
+        <v>0.007757454211569894</v>
       </c>
       <c r="X2" t="n">
-        <v>0.1505709306260574</v>
+        <v>0.1442376117527625</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.0153</v>
+        <v>0.0147</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.007565719120135449</v>
+        <v>0.00726789252404153</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.1593145516074449</v>
+        <v>0.1515973275987003</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.0144</v>
+        <v>0.0139</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.007194585448392445</v>
+        <v>0.006853525346735587</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.1690400676818949</v>
+        <v>0.1582344367660516</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.0138</v>
+        <v>0.0131</v>
       </c>
     </row>
     <row r="3">
@@ -2656,94 +2656,94 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.03349068322981388</v>
+        <v>0.03487175848735581</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08192407453416152</v>
+        <v>0.08818416403561558</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0475</v>
+        <v>0.05</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02367701863354015</v>
+        <v>0.02434282876299535</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1129573664596274</v>
+        <v>0.1188532441732558</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0391</v>
+        <v>0.0404</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01903773913043448</v>
+        <v>0.01952763844052862</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1332283975155281</v>
+        <v>0.1400675440774724</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0333</v>
+        <v>0.0343</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01611180124223574</v>
+        <v>0.01646386888502826</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1481260869565221</v>
+        <v>0.1554383766717471</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0291</v>
+        <v>0.0298</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01408198757763951</v>
+        <v>0.01445244598957195</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1612654906832303</v>
+        <v>0.1695651140515768</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0259</v>
+        <v>0.0266</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.01261316770186308</v>
+        <v>0.01295075384014995</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1725550062111808</v>
+        <v>0.1810835042037642</v>
       </c>
       <c r="S3" t="n">
-        <v>0.0235</v>
+        <v>0.0242</v>
       </c>
       <c r="T3" t="n">
-        <v>0.01151299378881971</v>
+        <v>0.0117476143176414</v>
       </c>
       <c r="U3" t="n">
-        <v>0.1830932670807461</v>
+        <v>0.1902516974706418</v>
       </c>
       <c r="V3" t="n">
-        <v>0.0217</v>
+        <v>0.0221</v>
       </c>
       <c r="W3" t="n">
-        <v>0.01059006211180099</v>
+        <v>0.0107825747632058</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1912322732919262</v>
+        <v>0.1987403277874324</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.0201</v>
+        <v>0.0205</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.009906608695652254</v>
+        <v>0.01002158288694105</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.2002406211180132</v>
+        <v>0.2072629855617419</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.0189</v>
+        <v>0.0191</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.009361490683229803</v>
+        <v>0.0093816737025092</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.2095461366459635</v>
+        <v>0.2145405761112474</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.0179</v>
+        <v>0.018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>